<commit_message>
Added another customer need and engineering requirement
</commit_message>
<xml_diff>
--- a/Ping Pong Buddy Needs and Engineering Requirements.xlsx
+++ b/Ping Pong Buddy Needs and Engineering Requirements.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nievec\Documents\RPI Senior Year\RCOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nievec\Documents\RPI Senior Year\RCOS\Ping-Pong-Buddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8650" windowHeight="3250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="Needs and Requirements" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Need #</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>The apparatus can use any color ball</t>
+  </si>
+  <si>
+    <t>Keep track of user progress</t>
+  </si>
+  <si>
+    <t>Track ball return placement</t>
+  </si>
+  <si>
+    <t>Needs to be accurate</t>
   </si>
 </sst>
 </file>
@@ -939,8 +948,8 @@
   <dimension ref="A1:T45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1630,12 +1639,16 @@
       <c r="A25" s="19">
         <v>10</v>
       </c>
-      <c r="B25" s="19"/>
+      <c r="B25" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="C25" s="19"/>
       <c r="D25" s="32">
         <v>10.1</v>
       </c>
-      <c r="E25" s="19"/>
+      <c r="E25" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="F25" s="11"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -1656,7 +1669,9 @@
       <c r="A26" s="11">
         <v>11</v>
       </c>
-      <c r="B26" s="11"/>
+      <c r="B26" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="C26" s="11"/>
       <c r="D26" s="31">
         <v>11.1</v>

</xml_diff>

<commit_message>
minor updates to customer needs and requirements
</commit_message>
<xml_diff>
--- a/Ping Pong Buddy Needs and Engineering Requirements.xlsx
+++ b/Ping Pong Buddy Needs and Engineering Requirements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936"/>
   </bookViews>
   <sheets>
     <sheet name="Needs and Requirements" sheetId="1" r:id="rId1"/>
@@ -947,28 +947,28 @@
   </sheetPr>
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="12"/>
-    <col min="2" max="2" width="52.7265625" customWidth="1"/>
-    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" style="32"/>
-    <col min="5" max="5" width="50.54296875" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="21.1796875" customWidth="1"/>
-    <col min="9" max="9" width="9.453125" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" customWidth="1"/>
-    <col min="11" max="11" width="25.453125" customWidth="1"/>
-    <col min="12" max="12" width="56.1796875" customWidth="1"/>
-    <col min="13" max="20" width="3.7265625" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="12"/>
+    <col min="2" max="2" width="52.77734375" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="32"/>
+    <col min="5" max="5" width="50.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" customWidth="1"/>
+    <col min="11" max="11" width="25.44140625" customWidth="1"/>
+    <col min="12" max="12" width="56.21875" customWidth="1"/>
+    <col min="13" max="20" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="74" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="73.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1060,7 +1060,7 @@
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
     </row>
-    <row r="3" spans="1:20" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1086,7 +1086,7 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1110,7 +1110,7 @@
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
     </row>
-    <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1134,7 +1134,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>2</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1186,7 +1186,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
     </row>
-    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1210,7 +1210,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" spans="1:20" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>3</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
     </row>
-    <row r="10" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1264,7 +1264,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>4</v>
       </c>
@@ -1294,7 +1294,7 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
     </row>
-    <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1320,7 +1320,7 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
     </row>
-    <row r="13" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1344,7 +1344,7 @@
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
     </row>
-    <row r="14" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1368,7 +1368,7 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>6</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>7</v>
       </c>
@@ -1428,7 +1428,7 @@
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1454,7 +1454,7 @@
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
       <c r="B18" s="6"/>
       <c r="C18" s="25"/>
@@ -1478,7 +1478,7 @@
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
     </row>
-    <row r="19" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>8</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="23"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
@@ -1532,7 +1532,7 @@
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
@@ -1556,7 +1556,7 @@
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
     </row>
-    <row r="22" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="32">
@@ -1579,7 +1579,7 @@
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
     </row>
-    <row r="23" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>9</v>
       </c>
@@ -1609,7 +1609,7 @@
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
       <c r="B24" s="6"/>
       <c r="C24" s="28"/>
@@ -1635,7 +1635,7 @@
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>10</v>
       </c>
@@ -1665,7 +1665,7 @@
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>11</v>
       </c>
@@ -1693,7 +1693,7 @@
       <c r="S26" s="12"/>
       <c r="T26" s="6"/>
     </row>
-    <row r="27" spans="1:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37">
         <v>12</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="S27" s="11"/>
       <c r="T27" s="11"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="38">
         <v>13</v>
       </c>
@@ -1745,22 +1745,22 @@
       <c r="S28" s="6"/>
       <c r="T28" s="6"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>23</v>
       </c>
@@ -1768,57 +1768,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
         <v>35</v>
       </c>
@@ -1840,13 +1840,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.26953125" customWidth="1"/>
-    <col min="2" max="2" width="54.7265625" customWidth="1"/>
+    <col min="1" max="1" width="50.21875" customWidth="1"/>
+    <col min="2" max="2" width="54.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>36</v>
       </c>
@@ -1854,22 +1854,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1877,42 +1877,42 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>

</xml_diff>